<commit_message>
Third iteration of tests - checking classification
</commit_message>
<xml_diff>
--- a/Final_Dissertation_Code/Unit_Tests/UnitTest.xlsx
+++ b/Final_Dissertation_Code/Unit_Tests/UnitTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Final Year Project\FYP Development\Final_Dissertation_Code\Unit_Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8EA8B1-EE3B-4241-9CE4-AAF0EE813658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938B6F24-B19C-4C92-9C37-9520B70917F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABE4211C-F3FD-442E-9380-AD90BAFA99B5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
   <si>
     <t>Test Run Date</t>
   </si>
@@ -186,6 +186,81 @@
   </si>
   <si>
     <t>score &gt; 70</t>
+  </si>
+  <si>
+    <t>test_class_person</t>
+  </si>
+  <si>
+    <t>check that the correct class is detected</t>
+  </si>
+  <si>
+    <t>classes = 1</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>test_class_chair</t>
+  </si>
+  <si>
+    <t>test_class_handbag</t>
+  </si>
+  <si>
+    <t>test_class_suitcase</t>
+  </si>
+  <si>
+    <t>test_class_keyboard</t>
+  </si>
+  <si>
+    <t>test_class_bottle</t>
+  </si>
+  <si>
+    <t>test_class_teddybear</t>
+  </si>
+  <si>
+    <t>test_class_phone</t>
+  </si>
+  <si>
+    <t>classes = 62</t>
+  </si>
+  <si>
+    <t>classes = 31</t>
+  </si>
+  <si>
+    <t>classes = 33</t>
+  </si>
+  <si>
+    <t>classes = 76</t>
+  </si>
+  <si>
+    <t>classes = 44</t>
+  </si>
+  <si>
+    <t>classes = 88</t>
+  </si>
+  <si>
+    <t>classes = 77</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>handbag</t>
+  </si>
+  <si>
+    <t>suitcase</t>
+  </si>
+  <si>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>bottle</t>
+  </si>
+  <si>
+    <t>teddy bear</t>
+  </si>
+  <si>
+    <t>cell phone</t>
   </si>
 </sst>
 </file>
@@ -583,11 +658,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A0DBF3-5FAB-4943-B769-AC3FDD8A7A6D}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,6 +1287,296 @@
         <v>20</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B22" s="5">
+        <v>6</v>
+      </c>
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B23" s="5">
+        <v>6</v>
+      </c>
+      <c r="C23" s="5">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B24" s="5">
+        <v>6</v>
+      </c>
+      <c r="C24" s="5">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B25" s="5">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B26" s="5">
+        <v>6</v>
+      </c>
+      <c r="C26" s="5">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B27" s="5">
+        <v>6</v>
+      </c>
+      <c r="C27" s="5">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B28" s="5">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>43884</v>
+      </c>
+      <c r="B29" s="16">
+        <v>6</v>
+      </c>
+      <c r="C29" s="16">
+        <v>22</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>43884</v>
+      </c>
+      <c r="B30" s="5">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5">
+        <v>15</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>43884</v>
+      </c>
+      <c r="B31" s="16">
+        <v>7</v>
+      </c>
+      <c r="C31" s="16">
+        <v>16</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
unittest conducted for distance sensor
</commit_message>
<xml_diff>
--- a/Final_Dissertation_Code/Unit_Tests/UnitTest.xlsx
+++ b/Final_Dissertation_Code/Unit_Tests/UnitTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Final Year Project\FYP Development\Final_Dissertation_Code\Unit_Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938B6F24-B19C-4C92-9C37-9520B70917F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC1B689-15AB-4035-90E2-AD49B56DEE31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABE4211C-F3FD-442E-9380-AD90BAFA99B5}"/>
+    <workbookView xWindow="13320" yWindow="1740" windowWidth="17280" windowHeight="8964" xr2:uid="{ABE4211C-F3FD-442E-9380-AD90BAFA99B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="91">
   <si>
     <t>Test Run Date</t>
   </si>
@@ -261,6 +261,51 @@
   </si>
   <si>
     <t>cell phone</t>
+  </si>
+  <si>
+    <t>test_long_distance_sensor</t>
+  </si>
+  <si>
+    <t>check the sensor detection from greater than 60 inches away</t>
+  </si>
+  <si>
+    <t>distance &gt;= 60 inches</t>
+  </si>
+  <si>
+    <t>check the sensor detection from less than 60 inches away</t>
+  </si>
+  <si>
+    <t>distance &lt; 60 inches</t>
+  </si>
+  <si>
+    <t>test_medium_distance_sensor</t>
+  </si>
+  <si>
+    <t>test_short_distance_sensor</t>
+  </si>
+  <si>
+    <t>check the sensor detection from greater than 20 inches away and less than 60 inches away</t>
+  </si>
+  <si>
+    <t>check the sensor detection from less than 20 inches away or greater than 60 inches away</t>
+  </si>
+  <si>
+    <t>check the sensor detection from less than 20 inches away</t>
+  </si>
+  <si>
+    <t>check the sensor detection from greater than 20 inches away</t>
+  </si>
+  <si>
+    <t>distance &gt;= 20 and &lt; 60</t>
+  </si>
+  <si>
+    <t>distance &lt; 20 or &gt; 60</t>
+  </si>
+  <si>
+    <t>distance &lt;= 20</t>
+  </si>
+  <si>
+    <t>distance &gt; 20</t>
   </si>
 </sst>
 </file>
@@ -304,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -321,11 +366,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -344,6 +400,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,11 +722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A0DBF3-5FAB-4943-B769-AC3FDD8A7A6D}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1577,6 +1641,209 @@
         <v>20</v>
       </c>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>43905</v>
+      </c>
+      <c r="B32" s="5">
+        <v>8</v>
+      </c>
+      <c r="C32" s="5">
+        <v>23</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>43905</v>
+      </c>
+      <c r="B33" s="16">
+        <v>8</v>
+      </c>
+      <c r="C33" s="16">
+        <v>24</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="19">
+        <v>43905</v>
+      </c>
+      <c r="B34" s="20">
+        <v>9</v>
+      </c>
+      <c r="C34" s="20">
+        <v>24</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>43905</v>
+      </c>
+      <c r="B35" s="5">
+        <v>10</v>
+      </c>
+      <c r="C35" s="5">
+        <v>25</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>43905</v>
+      </c>
+      <c r="B36" s="5">
+        <v>10</v>
+      </c>
+      <c r="C36" s="5">
+        <v>26</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>43905</v>
+      </c>
+      <c r="B37" s="5">
+        <v>10</v>
+      </c>
+      <c r="C37" s="5">
+        <v>27</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>43905</v>
+      </c>
+      <c r="B38" s="16">
+        <v>10</v>
+      </c>
+      <c r="C38" s="16">
+        <v>28</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>